<commit_message>
Exclui uns nomes repitidos
</commit_message>
<xml_diff>
--- a/Filtro.xlsx
+++ b/Filtro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="104">
   <si>
     <t xml:space="preserve">CODES</t>
   </si>
@@ -253,13 +253,7 @@
     <t xml:space="preserve">POLICLINICA MOVEL</t>
   </si>
   <si>
-    <t xml:space="preserve">FUNDACAO CASA 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNDACAO CASA 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNDACAO CASA 4</t>
+    <t xml:space="preserve">FUNDACAO CASA</t>
   </si>
   <si>
     <t xml:space="preserve">CENTRO DE MONITORAMENTO DA DENGUE  </t>
@@ -559,13 +553,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="67.38"/>
   </cols>
@@ -892,7 +886,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>78</v>
@@ -900,7 +894,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>79</v>
@@ -908,47 +902,47 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>85</v>
+      <c r="A46" s="3" t="n">
+        <v>2054035</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="2" t="s">
+      <c r="A47" s="3" t="n">
+        <v>3884937</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="n">
-        <v>2054035</v>
+        <v>2708701</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>88</v>
@@ -956,146 +950,130 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="n">
-        <v>3884937</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>89</v>
+        <v>2054035</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="n">
         <v>2708701</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="n">
+        <v>3331962</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="n">
+        <v>2708728</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="n">
-        <v>2054035</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="n">
-        <v>2708701</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
-        <v>3331962</v>
-      </c>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="5" t="s">
         <v>91</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="n">
-        <v>2708728</v>
+        <v>7001975</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
-        <v>93</v>
+      <c r="A55" s="5" t="n">
+        <v>7167067</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="n">
-        <v>7001975</v>
+      <c r="A56" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="n">
-        <v>7167067</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
+      <c r="A57" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="3" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
-        <v>20</v>
+      <c r="A59" s="3" t="n">
+        <v>7114354</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" s="6" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="n">
-        <v>7114354</v>
-      </c>
-      <c r="B61" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="2" t="s">
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="n">
+      <c r="A64" s="3" t="n">
         <v>2054035</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>88</v>
+      <c r="B64" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>